<commit_message>
Final changes after check
</commit_message>
<xml_diff>
--- a/parameter/0.raw.data/conductivity/conductivity.xlsx
+++ b/parameter/0.raw.data/conductivity/conductivity.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romana\Dropbox\01_LEEF2\07_manuals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainerkrug/Documents_Local/git/LEEF/LEEF.parameter/parameter/0.raw.data/conductivity/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689E3DB4-7DD0-DB4F-83F9-B732E9937287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10680"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21620" windowHeight="21540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,7 +132,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,15 +142,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -157,12 +164,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,185 +466,217 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.6796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A11" t="s">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A12" t="s">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A13" t="s">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A14" t="s">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A15" t="s">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A16" t="s">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A17" t="s">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A18" t="s">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A19" t="s">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A20" t="s">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A21" t="s">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A22" t="s">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A23" t="s">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A24" t="s">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A25" t="s">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A26" t="s">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A27" t="s">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A28" t="s">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A29" t="s">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A30" t="s">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A31" t="s">
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A32" t="s">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A33" t="s">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="B33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>